<commit_message>
bug in KVIK dyr samlet
</commit_message>
<xml_diff>
--- a/data/ab_lager.xlsx
+++ b/data/ab_lager.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27504"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,10 +15,21 @@
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -30,6 +41,15 @@
     <t>model_gruppe</t>
   </si>
   <si>
+    <t>ab_dyr</t>
+  </si>
+  <si>
+    <t>ab_stald</t>
+  </si>
+  <si>
+    <t>ab_lager</t>
+  </si>
+  <si>
     <t>toklimastald_smågrise</t>
   </si>
   <si>
@@ -67,22 +87,13 @@
   </si>
   <si>
     <t>kvæg_andre_hyppig</t>
-  </si>
-  <si>
-    <t>ab_dyr</t>
-  </si>
-  <si>
-    <t>ab_lager</t>
-  </si>
-  <si>
-    <t>ab_stald</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -399,28 +410,28 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>0.09</v>
@@ -432,9 +443,9 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>0.09</v>
@@ -446,9 +457,9 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>0.5</v>
@@ -460,9 +471,9 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>0.5</v>
@@ -474,9 +485,9 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>0.5</v>
@@ -488,9 +499,9 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>2.82</v>
@@ -502,9 +513,9 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>1.21</v>
@@ -516,9 +527,9 @@
         <v>1.76</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>1.21</v>
@@ -530,9 +541,9 @@
         <v>1.76</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>28.06</v>
@@ -544,9 +555,9 @@
         <v>33.18</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>28.06</v>
@@ -558,9 +569,9 @@
         <v>33.18</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>28.06</v>
@@ -572,9 +583,9 @@
         <v>33.18</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <v>28.06</v>
@@ -586,9 +597,9 @@
         <v>33.18</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B14">
         <v>28.06</v>

</xml_diff>